<commit_message>
removed double counting of sinter/pellet coke in fuel upstream
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_factory-ccs-bfcoke.xlsx
+++ b/data/steel/steel_simplified_factory-ccs-bfcoke.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557C8D81-479C-9D46-ABDD-3B40A73E171E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA167D20-95F9-6740-955C-8F1EA52E493D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="1260" windowWidth="26520" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="65">
   <si>
     <t>Inflow</t>
   </si>
@@ -815,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1487,7 +1487,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
         <v>33</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -1525,58 +1525,6 @@
         <v>39</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="6" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>